<commit_message>
Old changes that didn't get committed
</commit_message>
<xml_diff>
--- a/Labs/Lab06/Lab6Rubric_CS295N_2023.xlsx
+++ b/Labs/Lab06/Lab6Rubric_CS295N_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS295N-CourseMaterials\Labs\Lab06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/Labs/Lab06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF283CEF-14CD-43CA-BF71-A7EF7B1D3B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA25654-7C21-334D-A26D-ECAE5E3E41BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13848" yWindow="0" windowWidth="16776" windowHeight="16644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13840" yWindow="500" windowWidth="16780" windowHeight="16640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab3Rubric_CS295N" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -124,13 +124,16 @@
   </si>
   <si>
     <t>Not required</t>
+  </si>
+  <si>
+    <t>Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -315,6 +318,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -661,7 +672,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -684,6 +695,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1045,12 +1060,12 @@
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="44.296875" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1073,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999">
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1524,17 +1539,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C8BAC4-7C35-B64C-9C0F-AC9B3324E891}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="44.296875" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="6.5" customWidth="1"/>
+    <col min="4" max="4" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1553,22 +1570,36 @@
       <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:6">
+      <c r="A5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17.399999999999999">
+      <c r="E6" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1640,7 +1671,7 @@
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1736,21 +1767,37 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="28.8" customHeight="1">
+    <row r="27" spans="1:6" ht="28.75" customHeight="1">
       <c r="A27" s="13" t="s">
         <v>12</v>
       </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="15" t="s">
         <v>1</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F29" s="6"/>
     </row>
@@ -1913,28 +1960,44 @@
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1945,19 +2008,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="4" customFormat="1">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -1968,7 +2031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -1979,7 +2042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>27</v>
       </c>
@@ -1990,7 +2053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -2001,7 +2064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -2009,7 +2072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62" s="7" t="s">
         <v>4</v>
       </c>
@@ -2022,11 +2085,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
         <v>6</v>
       </c>
@@ -2083,6 +2146,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A51:E51"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>